<commit_message>
update tests for spectramax read
</commit_message>
<xml_diff>
--- a/test/inputs/spectramax.xlsx
+++ b/test/inputs/spectramax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2843907E-82B1-5E44-9FCB-E672872B151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7397356A-3A26-194E-B66F-07BE37DF2AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="880" windowWidth="18980" windowHeight="9440" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="18820" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Plate</t>
   </si>
@@ -72,18 +72,9 @@
     <t>spectramax</t>
   </si>
   <si>
-    <t>abs</t>
-  </si>
-  <si>
     <t>$GITHUB_WORKSPACE/test/inputs/spectramax-data.txt</t>
   </si>
   <si>
-    <t>535,(600 700)</t>
-  </si>
-  <si>
-    <t>600 700</t>
-  </si>
-  <si>
     <t>Channel</t>
   </si>
   <si>
@@ -94,6 +85,21 @@
   </si>
   <si>
     <t>New name</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>abs600</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>abs700</t>
+  </si>
+  <si>
+    <t>535_485,600,700</t>
   </si>
 </sst>
 </file>
@@ -135,9 +141,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -476,13 +481,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -493,7 +499,7 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
@@ -514,10 +520,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -537,7 +543,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,22 +553,27 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tests to use new spectramax data too
</commit_message>
<xml_diff>
--- a/test/inputs/spectramax.xlsx
+++ b/test/inputs/spectramax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7397356A-3A26-194E-B66F-07BE37DF2AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54870F4E-5255-374C-BA7E-9385576F9FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="18820" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="-30100" yWindow="920" windowWidth="29940" windowHeight="18580" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Plate</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>535_485,600,700</t>
+  </si>
+  <si>
+    <t>$GITHUB_WORKSPACE/test/inputs/spectramax-data2.txt</t>
+  </si>
+  <si>
+    <t>600,700,530_485,530_485_1,530_485_2</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -530,6 +536,17 @@
       </c>
       <c r="E2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spectramax parse bug (#61)
* parse channels in spectramax to fix duplicates

if absorbance channels specified as "600 700" in two separate tables, it means the first is 600 and second is 700
for fluorescence it probably just means multiple gains were used

* update tests for spectramax read

* added extra spectramax data for tests

* simplify duplicate channel catch for coverage

since the break always triggers, coverage will treat the end of the for loop and a line that wasnt reached

* append to the first duplicate fluorescence too

* empty cells can get in the way of parsing

the exact position depends on the number of wavelengths that are read?
at least removing empty cells realigns both test data

* update tests to use new spectramax data too

* fix test mistakes
</commit_message>
<xml_diff>
--- a/test/inputs/spectramax.xlsx
+++ b/test/inputs/spectramax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2843907E-82B1-5E44-9FCB-E672872B151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600C3CC6-20CE-C444-810B-B297372D9F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="880" windowWidth="18980" windowHeight="9440" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="-30100" yWindow="920" windowWidth="29940" windowHeight="18580" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Plate</t>
   </si>
@@ -72,18 +72,9 @@
     <t>spectramax</t>
   </si>
   <si>
-    <t>abs</t>
-  </si>
-  <si>
     <t>$GITHUB_WORKSPACE/test/inputs/spectramax-data.txt</t>
   </si>
   <si>
-    <t>535,(600 700)</t>
-  </si>
-  <si>
-    <t>600 700</t>
-  </si>
-  <si>
     <t>Channel</t>
   </si>
   <si>
@@ -94,6 +85,27 @@
   </si>
   <si>
     <t>New name</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>abs600</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>abs700</t>
+  </si>
+  <si>
+    <t>535_485,600,700</t>
+  </si>
+  <si>
+    <t>$GITHUB_WORKSPACE/test/inputs/spectramax-data2.txt</t>
+  </si>
+  <si>
+    <t>600,700,530_485_1,530_485_2,530_485_3</t>
   </si>
 </sst>
 </file>
@@ -135,9 +147,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -473,16 +484,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -493,7 +505,7 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
@@ -514,16 +526,33 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -537,7 +566,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,22 +576,27 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +671,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>